<commit_message>
updates to bsdf models based on Eric's changes
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Base Data Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Base Data Model.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a\git\Beiersdorf\seeddata-bsdf\99-exceldmd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/Beiersdorf/seeddata-bsdf/99-exceldmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_Attribute_Display_Types">'[1]20170320 065838_DataModel_Templ'!#REF!</definedName>
     <definedName name="_Attribute_Name">'[1]S7 - Attribute'!$E$2:$E$1048576</definedName>
     <definedName name="_Boolean">'[1]20170320 065838_DataModel_Templ'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ATTRIBUTES!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ATTRIBUTES!$A$1:$V$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ENTITIES!$A$1:$D$1</definedName>
     <definedName name="_RefDataAttribute">ATTRIBUTES!#REF!</definedName>
@@ -46,8 +46,8 @@
   </definedNames>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -67,7 +67,7 @@
     <author>Eric Sambach</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="1" shapeId="0">
+    <comment ref="B6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="517">
   <si>
     <t>ACTION</t>
   </si>
@@ -1706,12 +1706,24 @@
   </si>
   <si>
     <t>sspgrproduct</t>
+  </si>
+  <si>
+    <t>NestedGrid</t>
+  </si>
+  <si>
+    <t>alastmodifieddate</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Last Modified Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
@@ -2041,11 +2053,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="18"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="18" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="0" xfId="19" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -2069,27 +2081,7 @@
     <cellStyle name="Neutral" xfId="18" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2624,7 +2616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C34"/>
@@ -2633,84 +2625,84 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="87.625" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="45"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="48"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="48"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="45"/>
+      <c r="C5" s="48"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="48"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="48"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="45"/>
+      <c r="C8" s="48"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
@@ -2879,12 +2871,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
+      <selection activeCell="B34" sqref="B34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
       <selection activeCell="A5" sqref="A5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
-      <selection activeCell="B34" sqref="B34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -2905,7 +2897,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9"/>
+  <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2913,17 +2905,17 @@
       <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3111,12 +3103,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3129,20 +3121,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A4:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3291,11 +3283,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -3313,12 +3305,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="32" customWidth="1"/>
     <col min="3" max="3" width="29" style="26" customWidth="1"/>
-    <col min="4" max="4" width="26.125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" style="26" customWidth="1"/>
     <col min="5" max="16384" width="11" style="26"/>
   </cols>
   <sheetData>
@@ -3483,7 +3475,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3491,12 +3483,12 @@
       <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,14 +3531,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -3557,43 +3549,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AG109"/>
+  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:AG110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="38.875" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="38.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="27" customWidth="1"/>
-    <col min="9" max="9" width="22.125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="26.125" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" style="26" customWidth="1"/>
+    <col min="12" max="12" width="26.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.875" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.875" style="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.125" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="12.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.875" style="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="7.125" style="26"/>
+    <col min="21" max="21" width="17.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="7.1640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3661,7 +3653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="25" t="s">
         <v>351</v>
       </c>
@@ -3687,7 +3679,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="44" t="s">
         <v>352</v>
       </c>
@@ -3710,7 +3702,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B4" s="26" t="s">
         <v>353</v>
       </c>
@@ -3727,7 +3719,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
         <v>354</v>
       </c>
@@ -3744,7 +3736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B6" s="26" t="s">
         <v>366</v>
       </c>
@@ -3764,7 +3756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B7" s="26" t="s">
         <v>368</v>
       </c>
@@ -3781,7 +3773,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B8" s="26" t="s">
         <v>370</v>
       </c>
@@ -3798,7 +3790,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
         <v>373</v>
       </c>
@@ -3815,7 +3807,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B10" s="26" t="s">
         <v>375</v>
       </c>
@@ -3832,7 +3824,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
         <v>233</v>
       </c>
@@ -3858,7 +3850,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B12" s="25" t="s">
         <v>377</v>
       </c>
@@ -3875,7 +3867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
         <v>380</v>
       </c>
@@ -3892,7 +3884,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B14" s="26" t="s">
         <v>382</v>
       </c>
@@ -3921,7 +3913,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B15" s="26" t="s">
         <v>228</v>
       </c>
@@ -3938,7 +3930,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B16" s="26" t="s">
         <v>261</v>
       </c>
@@ -3967,7 +3959,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
         <v>260</v>
       </c>
@@ -3996,7 +3988,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
         <v>258</v>
       </c>
@@ -4025,7 +4017,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
         <v>259</v>
       </c>
@@ -4054,7 +4046,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="26" t="s">
         <v>226</v>
       </c>
@@ -4071,7 +4063,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="26" t="s">
         <v>349</v>
       </c>
@@ -4088,7 +4080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="26" t="s">
         <v>234</v>
       </c>
@@ -4104,8 +4096,11 @@
       <c r="F22" s="26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="26" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="26" t="s">
         <v>236</v>
       </c>
@@ -4128,7 +4123,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="s">
         <v>235</v>
       </c>
@@ -4145,7 +4140,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="25" t="s">
         <v>229</v>
       </c>
@@ -4162,7 +4157,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="25" t="s">
         <v>230</v>
       </c>
@@ -4179,7 +4174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="s">
         <v>302</v>
       </c>
@@ -4205,7 +4200,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
         <v>385</v>
       </c>
@@ -4222,7 +4217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="25" t="s">
         <v>387</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>389</v>
       </c>
@@ -4256,7 +4251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
         <v>391</v>
       </c>
@@ -4273,7 +4268,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="26" t="s">
         <v>393</v>
       </c>
@@ -4290,7 +4285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="25" t="s">
         <v>395</v>
       </c>
@@ -4307,7 +4302,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="25" t="s">
         <v>397</v>
       </c>
@@ -4324,7 +4319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="25" t="s">
         <v>399</v>
       </c>
@@ -4341,7 +4336,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="25" t="s">
         <v>401</v>
       </c>
@@ -4358,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="25" t="s">
         <v>403</v>
       </c>
@@ -4375,7 +4370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="25" t="s">
         <v>405</v>
       </c>
@@ -4392,7 +4387,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="25" t="s">
         <v>408</v>
       </c>
@@ -4409,7 +4404,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="25" t="s">
         <v>410</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="25" t="s">
         <v>412</v>
       </c>
@@ -4443,7 +4438,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="25" t="s">
         <v>414</v>
       </c>
@@ -4460,7 +4455,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="25" t="s">
         <v>416</v>
       </c>
@@ -4477,7 +4472,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="26" t="s">
         <v>227</v>
       </c>
@@ -4494,7 +4489,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="25" t="s">
         <v>418</v>
       </c>
@@ -4511,7 +4506,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="25" t="s">
         <v>420</v>
       </c>
@@ -4528,7 +4523,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="25" t="s">
         <v>422</v>
       </c>
@@ -4545,7 +4540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="25" t="s">
         <v>424</v>
       </c>
@@ -4562,7 +4557,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="25" t="s">
         <v>426</v>
       </c>
@@ -4579,7 +4574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="25" t="s">
         <v>428</v>
       </c>
@@ -4596,7 +4591,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="25" t="s">
         <v>430</v>
       </c>
@@ -4613,7 +4608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="25" t="s">
         <v>432</v>
       </c>
@@ -4630,7 +4625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="26" t="s">
         <v>434</v>
       </c>
@@ -4647,7 +4642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="26" t="s">
         <v>436</v>
       </c>
@@ -4664,7 +4659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="26" t="s">
         <v>237</v>
       </c>
@@ -4680,8 +4675,11 @@
       <c r="F55" s="26" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="26" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="26" t="s">
         <v>238</v>
       </c>
@@ -4698,7 +4696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="26" t="s">
         <v>239</v>
       </c>
@@ -4715,7 +4713,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="26" t="s">
         <v>240</v>
       </c>
@@ -4732,7 +4730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="26" t="s">
         <v>241</v>
       </c>
@@ -4749,7 +4747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="26" t="s">
         <v>242</v>
       </c>
@@ -4766,7 +4764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="26" t="s">
         <v>243</v>
       </c>
@@ -4783,7 +4781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="26" t="s">
         <v>244</v>
       </c>
@@ -4800,7 +4798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="26" t="s">
         <v>245</v>
       </c>
@@ -4817,7 +4815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="26" t="s">
         <v>246</v>
       </c>
@@ -4834,7 +4832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="26" t="s">
         <v>247</v>
       </c>
@@ -4851,7 +4849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" s="26" t="s">
         <v>248</v>
       </c>
@@ -4868,7 +4866,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="26" t="s">
         <v>250</v>
       </c>
@@ -4885,7 +4883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="26" t="s">
         <v>249</v>
       </c>
@@ -4902,7 +4900,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="26" t="s">
         <v>251</v>
       </c>
@@ -4919,7 +4917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="26" t="s">
         <v>252</v>
       </c>
@@ -4936,7 +4934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71" s="26" t="s">
         <v>253</v>
       </c>
@@ -4953,7 +4951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="26" t="s">
         <v>254</v>
       </c>
@@ -4970,7 +4968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="26" t="s">
         <v>255</v>
       </c>
@@ -4987,7 +4985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="26" t="s">
         <v>256</v>
       </c>
@@ -5004,7 +5002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B75" s="26" t="s">
         <v>257</v>
       </c>
@@ -5021,7 +5019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="25" t="s">
         <v>438</v>
       </c>
@@ -5038,7 +5036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="25" t="s">
         <v>440</v>
       </c>
@@ -5055,7 +5053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B78" s="25" t="s">
         <v>442</v>
       </c>
@@ -5072,7 +5070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B79" s="25" t="s">
         <v>444</v>
       </c>
@@ -5089,7 +5087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B80" s="25" t="s">
         <v>446</v>
       </c>
@@ -5106,7 +5104,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B81" s="25" t="s">
         <v>448</v>
       </c>
@@ -5123,7 +5121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B82" s="25" t="s">
         <v>450</v>
       </c>
@@ -5140,7 +5138,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B83" s="25" t="s">
         <v>452</v>
       </c>
@@ -5157,7 +5155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B84" s="25" t="s">
         <v>454</v>
       </c>
@@ -5174,7 +5172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B85" s="25" t="s">
         <v>231</v>
       </c>
@@ -5191,7 +5189,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B86" s="25" t="s">
         <v>455</v>
       </c>
@@ -5208,7 +5206,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B87" s="25" t="s">
         <v>457</v>
       </c>
@@ -5225,7 +5223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B88" s="25" t="s">
         <v>459</v>
       </c>
@@ -5242,7 +5240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B89" s="25" t="s">
         <v>461</v>
       </c>
@@ -5259,7 +5257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B90" s="25" t="s">
         <v>463</v>
       </c>
@@ -5276,7 +5274,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B91" s="25" t="s">
         <v>465</v>
       </c>
@@ -5293,7 +5291,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B92" s="25" t="s">
         <v>467</v>
       </c>
@@ -5310,7 +5308,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B93" s="25" t="s">
         <v>468</v>
       </c>
@@ -5327,7 +5325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B94" s="25" t="s">
         <v>470</v>
       </c>
@@ -5344,7 +5342,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B95" s="25" t="s">
         <v>472</v>
       </c>
@@ -5361,7 +5359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B96" s="25" t="s">
         <v>474</v>
       </c>
@@ -5378,7 +5376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="25" t="s">
         <v>476</v>
       </c>
@@ -5395,7 +5393,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" s="25" t="s">
         <v>478</v>
       </c>
@@ -5412,7 +5410,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="25" t="s">
         <v>480</v>
       </c>
@@ -5429,7 +5427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="26" t="s">
         <v>482</v>
       </c>
@@ -5445,8 +5443,11 @@
       <c r="F100" s="26" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G100" s="26" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" s="26" t="s">
         <v>484</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="26" t="s">
         <v>486</v>
       </c>
@@ -5480,7 +5481,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" s="26" t="s">
         <v>488</v>
       </c>
@@ -5497,7 +5498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="26" t="s">
         <v>490</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="26" t="s">
         <v>492</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="26" t="s">
         <v>494</v>
       </c>
@@ -5548,7 +5549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="26" t="s">
         <v>496</v>
       </c>
@@ -5565,7 +5566,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="26" t="s">
         <v>498</v>
       </c>
@@ -5582,7 +5583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="39" t="s">
         <v>500</v>
       </c>
@@ -5602,12 +5603,29 @@
         <v>502</v>
       </c>
     </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="F110" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>378</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:V1"/>
+  <autoFilter ref="A1:V109"/>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -5615,9 +5633,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -5628,22 +5646,22 @@
   </customSheetViews>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B4:B5 B1 B110:B1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F5 G4:G5">
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="18" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14 B13:B14">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:B17 B39:B108">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -5655,7 +5673,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5663,22 +5681,22 @@
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.125" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.875" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" style="26" customWidth="1"/>
     <col min="9" max="9" width="22.5" style="26" customWidth="1"/>
-    <col min="10" max="10" width="15.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="26"/>
+    <col min="10" max="10" width="15.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5713,7 +5731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>268</v>
       </c>
@@ -5737,7 +5755,7 @@
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
     </row>
-    <row r="3" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>269</v>
       </c>
@@ -5763,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>270</v>
       </c>
@@ -5783,7 +5801,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>271</v>
       </c>
@@ -5806,7 +5824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
         <v>271</v>
       </c>
@@ -5832,7 +5850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="26" t="s">
         <v>272</v>
       </c>
@@ -5855,7 +5873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="26" t="s">
         <v>273</v>
       </c>
@@ -5877,14 +5895,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -5896,48 +5914,48 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AA82"/>
+  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:AA85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.625" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.625" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.125" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="39" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.625" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="39" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.125" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" style="39" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" style="39" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.625" style="39" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" style="39" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.875" style="39" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" style="39" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" style="39" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.875" style="39" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" style="39" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.125" style="39" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.83203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" style="39" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="12.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.625" style="39" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.875" style="39" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.83203125" style="39" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="11" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -6020,14 +6038,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2" s="39" t="s">
         <v>225</v>
       </c>
       <c r="D2" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K2" s="39" t="s">
@@ -6037,14 +6055,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B3" s="39" t="s">
         <v>225</v>
       </c>
       <c r="D3" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K3" s="39" t="s">
@@ -6054,55 +6072,55 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B4" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="45" t="s">
         <v>354</v>
       </c>
       <c r="O4" s="39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="46" t="s">
         <v>352</v>
       </c>
       <c r="P5" s="25" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B6" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="45" t="s">
         <v>351</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B7" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B8" s="39" t="s">
         <v>224</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K8" s="39" t="s">
@@ -6112,14 +6130,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B9" s="39" t="s">
         <v>224</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K9" s="39" t="s">
@@ -6129,7 +6147,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B10" s="39" t="s">
         <v>224</v>
       </c>
@@ -6137,7 +6155,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
         <v>224</v>
       </c>
@@ -6145,7 +6163,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B12" s="39" t="s">
         <v>224</v>
       </c>
@@ -6153,7 +6171,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="39" t="s">
         <v>224</v>
       </c>
@@ -6161,7 +6179,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="39" t="s">
         <v>224</v>
       </c>
@@ -6169,7 +6187,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="39" t="s">
         <v>224</v>
       </c>
@@ -6177,7 +6195,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B16" s="39" t="s">
         <v>224</v>
       </c>
@@ -6185,7 +6203,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="39" t="s">
         <v>224</v>
       </c>
@@ -6193,7 +6211,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="39" t="s">
         <v>224</v>
       </c>
@@ -6201,7 +6219,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="39" t="s">
         <v>224</v>
       </c>
@@ -6209,7 +6227,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="39" t="s">
         <v>224</v>
       </c>
@@ -6220,7 +6238,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="39" t="s">
         <v>224</v>
       </c>
@@ -6231,7 +6249,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="39" t="s">
         <v>224</v>
       </c>
@@ -6245,7 +6263,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="39" t="s">
         <v>224</v>
       </c>
@@ -6259,7 +6277,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="39" t="s">
         <v>224</v>
       </c>
@@ -6270,18 +6288,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="45" t="s">
         <v>354</v>
       </c>
       <c r="O25" s="39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="39" t="s">
         <v>224</v>
       </c>
@@ -6289,7 +6307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="39" t="s">
         <v>224</v>
       </c>
@@ -6297,7 +6315,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="39" t="s">
         <v>224</v>
       </c>
@@ -6305,7 +6323,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="39" t="s">
         <v>224</v>
       </c>
@@ -6313,7 +6331,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="39" t="s">
         <v>224</v>
       </c>
@@ -6321,37 +6339,37 @@
         <v>393</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="46" t="s">
         <v>352</v>
       </c>
       <c r="P31" s="25" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="45" t="s">
         <v>351</v>
       </c>
       <c r="P32" s="39" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="39" t="s">
         <v>224</v>
       </c>
@@ -6359,7 +6377,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="39" t="s">
         <v>224</v>
       </c>
@@ -6367,7 +6385,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="39" t="s">
         <v>224</v>
       </c>
@@ -6375,7 +6393,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="39" t="s">
         <v>224</v>
       </c>
@@ -6383,7 +6401,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="39" t="s">
         <v>224</v>
       </c>
@@ -6391,7 +6409,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="39" t="s">
         <v>224</v>
       </c>
@@ -6399,7 +6417,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="39" t="s">
         <v>224</v>
       </c>
@@ -6407,7 +6425,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="39" t="s">
         <v>224</v>
       </c>
@@ -6415,7 +6433,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="39" t="s">
         <v>224</v>
       </c>
@@ -6423,7 +6441,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="39" t="s">
         <v>224</v>
       </c>
@@ -6431,7 +6449,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="39" t="s">
         <v>224</v>
       </c>
@@ -6439,7 +6457,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="39" t="s">
         <v>224</v>
       </c>
@@ -6447,7 +6465,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="39" t="s">
         <v>224</v>
       </c>
@@ -6455,7 +6473,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="39" t="s">
         <v>224</v>
       </c>
@@ -6463,7 +6481,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="39" t="s">
         <v>224</v>
       </c>
@@ -6471,7 +6489,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" s="39" t="s">
         <v>224</v>
       </c>
@@ -6479,7 +6497,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B50" s="39" t="s">
         <v>224</v>
       </c>
@@ -6487,7 +6505,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" s="39" t="s">
         <v>224</v>
       </c>
@@ -6495,7 +6513,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B52" s="39" t="s">
         <v>224</v>
       </c>
@@ -6503,7 +6521,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B53" s="39" t="s">
         <v>224</v>
       </c>
@@ -6511,7 +6529,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" s="39" t="s">
         <v>224</v>
       </c>
@@ -6519,7 +6537,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" s="39" t="s">
         <v>224</v>
       </c>
@@ -6527,7 +6545,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" s="39" t="s">
         <v>224</v>
       </c>
@@ -6535,7 +6553,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B57" s="39" t="s">
         <v>224</v>
       </c>
@@ -6543,7 +6561,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B58" s="39" t="s">
         <v>224</v>
       </c>
@@ -6551,7 +6569,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B59" s="39" t="s">
         <v>224</v>
       </c>
@@ -6559,7 +6577,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B60" s="39" t="s">
         <v>224</v>
       </c>
@@ -6567,14 +6585,14 @@
         <v>480</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B61" s="39" t="s">
         <v>223</v>
       </c>
       <c r="D61" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="F61" s="49" t="s">
+      <c r="F61" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K61" s="39" t="s">
@@ -6584,14 +6602,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B62" s="39" t="s">
         <v>223</v>
       </c>
       <c r="D62" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="G62" s="49" t="s">
+      <c r="G62" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K62" s="39" t="s">
@@ -6601,7 +6619,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B63" s="39" t="s">
         <v>223</v>
       </c>
@@ -6609,7 +6627,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B64" s="39" t="s">
         <v>223</v>
       </c>
@@ -6617,48 +6635,48 @@
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B65" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D65" s="47" t="s">
+      <c r="D65" s="45" t="s">
         <v>354</v>
       </c>
       <c r="O65" s="39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B66" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D66" s="48" t="s">
+      <c r="D66" s="46" t="s">
         <v>352</v>
       </c>
       <c r="P66" s="25" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B67" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D67" s="47" t="s">
+      <c r="D67" s="45" t="s">
         <v>351</v>
       </c>
       <c r="P67" s="39" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B68" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D68" s="47" t="s">
+      <c r="D68" s="45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B69" s="39" t="s">
         <v>223</v>
       </c>
@@ -6666,7 +6684,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B70" s="39" t="s">
         <v>223</v>
       </c>
@@ -6674,7 +6692,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B71" s="39" t="s">
         <v>223</v>
       </c>
@@ -6682,7 +6700,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B72" s="39" t="s">
         <v>223</v>
       </c>
@@ -6690,7 +6708,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B73" s="39" t="s">
         <v>223</v>
       </c>
@@ -6698,7 +6716,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B74" s="39" t="s">
         <v>223</v>
       </c>
@@ -6706,7 +6724,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B75" s="39" t="s">
         <v>223</v>
       </c>
@@ -6714,7 +6732,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B76" s="39" t="s">
         <v>223</v>
       </c>
@@ -6722,7 +6740,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B77" s="39" t="s">
         <v>223</v>
       </c>
@@ -6730,7 +6748,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B78" s="39" t="s">
         <v>223</v>
       </c>
@@ -6738,7 +6756,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B79" s="39" t="s">
         <v>223</v>
       </c>
@@ -6746,7 +6764,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B80" s="39" t="s">
         <v>223</v>
       </c>
@@ -6754,7 +6772,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="39" t="s">
         <v>223</v>
       </c>
@@ -6762,12 +6780,36 @@
         <v>511</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="39" t="s">
         <v>223</v>
       </c>
       <c r="D82" s="39" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" s="39" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B84" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="D84" s="39" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B85" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" s="39" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -6779,6 +6821,12 @@
     <sortCondition ref="D2:D82"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6789,12 +6837,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D4:D5">
@@ -6846,7 +6888,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6854,15 +6896,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7358,12 +7400,12 @@
     <sortCondition ref="B2:B41"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7376,7 +7418,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7384,23 +7426,23 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" customWidth="1"/>
-    <col min="11" max="11" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7472,12 +7514,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Datamodel, removed filters (no data change)
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Base Data Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Base Data Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -46,8 +46,8 @@
   </definedNames>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -2764,9 +2764,9 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="18"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="18" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="0" xfId="19" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="18" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="18" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -3605,73 +3605,73 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="49"/>
+      <c r="C1" s="50"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="48"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="48"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="48"/>
+      <c r="C5" s="49"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="49"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="49"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="49"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
@@ -3840,12 +3840,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
+      <selection activeCell="A5" sqref="A5"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
       <selection activeCell="B34" sqref="B34"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
-      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4072,12 +4072,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4252,11 +4252,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4500,14 +4500,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4518,14 +4518,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" filterMode="1"/>
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AG229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B205" sqref="B6:B205"/>
+      <selection pane="bottomRight" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4622,7 +4622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="25" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>349</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="25" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="44" t="s">
         <v>350</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>351</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>352</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>502</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>260</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>259</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>257</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>258</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>226</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>347</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>235</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>234</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
         <v>300</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>403</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="25" t="s">
         <v>406</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="25" t="s">
         <v>408</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
         <v>410</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="25" t="s">
         <v>412</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="25" t="s">
         <v>414</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
         <v>227</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
         <v>416</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="25" t="s">
         <v>418</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="25" t="s">
         <v>420</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
         <v>422</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="25" t="s">
         <v>424</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="25" t="s">
         <v>426</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="25" t="s">
         <v>428</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="25" t="s">
         <v>430</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="26" t="s">
         <v>432</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="26" t="s">
         <v>434</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="26" t="s">
         <v>236</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="56" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
         <v>237</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
         <v>238</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="26" t="s">
         <v>239</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
         <v>240</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
         <v>241</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
         <v>242</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
         <v>243</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
         <v>244</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="26" t="s">
         <v>245</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
         <v>246</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="26" t="s">
         <v>247</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="26" t="s">
         <v>249</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="26" t="s">
         <v>248</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="26" t="s">
         <v>250</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="26" t="s">
         <v>251</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="26" t="s">
         <v>252</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="26" t="s">
         <v>253</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="26" t="s">
         <v>254</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="26" t="s">
         <v>255</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="26" t="s">
         <v>256</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="25" t="s">
         <v>436</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="25" t="s">
         <v>438</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="25" t="s">
         <v>440</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="25" t="s">
         <v>442</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="25" t="s">
         <v>444</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="25" t="s">
         <v>446</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="25" t="s">
         <v>448</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="25" t="s">
         <v>450</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="25" t="s">
         <v>452</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="25" t="s">
         <v>231</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="25" t="s">
         <v>453</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="25" t="s">
         <v>455</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="25" t="s">
         <v>457</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="25" t="s">
         <v>459</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="25" t="s">
         <v>461</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="25" t="s">
         <v>463</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="25" t="s">
         <v>465</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="25" t="s">
         <v>466</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="25" t="s">
         <v>468</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="25" t="s">
         <v>470</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="25" t="s">
         <v>472</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B97" s="25" t="s">
         <v>474</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B98" s="25" t="s">
         <v>476</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B99" s="25" t="s">
         <v>478</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B100" s="26" t="s">
         <v>480</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B101" s="26" t="s">
         <v>482</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B102" s="26" t="s">
         <v>484</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B103" s="26" t="s">
         <v>486</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B104" s="26" t="s">
         <v>488</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B105" s="26" t="s">
         <v>490</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B106" s="26" t="s">
         <v>492</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B107" s="26" t="s">
         <v>494</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B108" s="26" t="s">
         <v>496</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B110" s="26" t="s">
         <v>512</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="26" t="s">
         <v>566</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="26" t="s">
         <v>566</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="26" t="s">
         <v>566</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
         <v>566</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="26" t="s">
         <v>566</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="26" t="s">
         <v>566</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="26" t="s">
         <v>566</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="26" t="s">
         <v>566</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="26" t="s">
         <v>566</v>
       </c>
@@ -6978,7 +6978,7 @@
       </c>
       <c r="I130" s="27"/>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B131" s="26" t="s">
         <v>750</v>
       </c>
@@ -6996,7 +6996,7 @@
       </c>
       <c r="I131" s="27"/>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B132" s="26" t="s">
         <v>749</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="26" t="s">
         <v>566</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="26" t="s">
         <v>566</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="26" t="s">
         <v>566</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="26" t="s">
         <v>566</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="26" t="s">
         <v>566</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="26" t="s">
         <v>566</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
         <v>566</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
         <v>566</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="26" t="s">
         <v>566</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="26" t="s">
         <v>566</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="26" t="s">
         <v>566</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="26" t="s">
         <v>566</v>
       </c>
@@ -7456,7 +7456,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="26" t="s">
         <v>566</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="26" t="s">
         <v>566</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="26" t="s">
         <v>566</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="26" t="s">
         <v>566</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="26" t="s">
         <v>566</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="26" t="s">
         <v>566</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="26" t="s">
         <v>566</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="26" t="s">
         <v>566</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="26" t="s">
         <v>566</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="26" t="s">
         <v>566</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="26" t="s">
         <v>566</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="26" t="s">
         <v>566</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="26" t="s">
         <v>566</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="26" t="s">
         <v>566</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="26" t="s">
         <v>566</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="26" t="s">
         <v>566</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="26" t="s">
         <v>566</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="26" t="s">
         <v>566</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="26" t="s">
         <v>566</v>
       </c>
@@ -8410,7 +8410,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B206" s="26" t="s">
         <v>705</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B207" s="26" t="s">
         <v>706</v>
       </c>
@@ -8448,7 +8448,7 @@
       </c>
       <c r="J207" s="27"/>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B208" s="26" t="s">
         <v>708</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="209" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B209" s="26" t="s">
         <v>710</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="210" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B210" s="26" t="s">
         <v>712</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="211" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B211" s="26" t="s">
         <v>714</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="212" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B212" s="26" t="s">
         <v>717</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B213" s="26" t="s">
         <v>719</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="214" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B214" s="26" t="s">
         <v>722</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B215" s="26" t="s">
         <v>724</v>
       </c>
@@ -8584,7 +8584,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="216" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B216" s="26" t="s">
         <v>726</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="217" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B217" s="26" t="s">
         <v>728</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="218" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B218" s="26" t="s">
         <v>730</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="219" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" s="26" t="s">
         <v>732</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="220" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B220" s="26" t="s">
         <v>734</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="221" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B221" s="26" t="s">
         <v>736</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="222" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B222" s="26" t="s">
         <v>737</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="223" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B223" s="26" t="s">
         <v>738</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="224" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B224" s="26" t="s">
         <v>739</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B225" s="26" t="s">
         <v>740</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B226" s="26" t="s">
         <v>742</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B227" s="26" t="s">
         <v>743</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="26" t="s">
         <v>566</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="26" t="s">
         <v>566</v>
       </c>
@@ -8829,21 +8829,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V229">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Marketing Basic"/>
-        <filter val="Marketing Website"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:V229"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -8851,9 +8841,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -9182,14 +9172,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -9204,8 +9194,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AA158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
@@ -9363,7 +9353,7 @@
       <c r="B4" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="48" t="s">
         <v>512</v>
       </c>
     </row>
@@ -9758,7 +9748,7 @@
       <c r="B47" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="48" t="s">
         <v>512</v>
       </c>
     </row>
@@ -10433,7 +10423,7 @@
       <c r="B128" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="D128" s="50" t="s">
+      <c r="D128" s="48" t="s">
         <v>512</v>
       </c>
     </row>
@@ -10947,12 +10937,6 @@
     <sortCondition ref="D2:D160"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
-    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10963,6 +10947,12 @@
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D4:D5">
@@ -11535,12 +11525,12 @@
     <sortCondition ref="B2:B41"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11649,12 +11639,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11677,65 +11667,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF273DB610BE64D8338C714685CCF46" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2352d1590348b4df6d1de565ccbd102a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fff5a07-2326-481b-a4e9-87ff7a79f8dd" xmlns:ns3="2e2046eb-f52d-433a-aad8-97c651e3992c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5c0a0cba47b5c64de8255dd546e4ec9" ns2:_="" ns3:_="">
     <xsd:import namespace="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
@@ -11913,6 +11844,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
   <ds:schemaRefs>
@@ -11931,22 +11921,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAC4C16-FDF5-437E-A8C4-D650CA39502E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11963,4 +11937,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>